<commit_message>
fix: Modify download template prompt
--bug=1054044 --user=王孝刚 【知识库】上传文档-QA问答对-下载Excel/CSV模版-显示问题答案最长不超过4096个字符，实际上可以导入超过4096个字符的数据 https://www.tapd.cn/57709429/s/1677605
</commit_message>
<xml_diff>
--- a/apps/dataset/template/excel_template_en.xlsx
+++ b/apps/dataset/template/excel_template_en.xlsx
@@ -33,7 +33,7 @@
     <t>Section title (optional)</t>
   </si>
   <si>
-    <t>Section content (required, question answer, no more than 4096 characters)</t>
+    <t>Section content (required, question answer)</t>
   </si>
   <si>
     <t>Question (optional, one per line in the cell)</t>
@@ -1227,7 +1227,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>

</xml_diff>